<commit_message>
F*ck nhẹ deadline :|
</commit_message>
<xml_diff>
--- a/KH_HUE_T07_DatabaseDesign_v1.0.xlsx
+++ b/KH_HUE_T07_DatabaseDesign_v1.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="67">
   <si>
     <t>PHIENDAUGIA</t>
   </si>
@@ -197,6 +197,24 @@
   </si>
   <si>
     <t>Yes/No</t>
+  </si>
+  <si>
+    <t>CUOCDAUGIA</t>
+  </si>
+  <si>
+    <t>ThoiDiem</t>
+  </si>
+  <si>
+    <t>GiaDuocDat</t>
+  </si>
+  <si>
+    <t>Bảng CUOCDAUGIA (CUỘC ĐẤU GIÁ)</t>
+  </si>
+  <si>
+    <t>Thời điểm đấu giá</t>
+  </si>
+  <si>
+    <t>Giá được đặt</t>
   </si>
 </sst>
 </file>
@@ -378,6 +396,100 @@
         <a:xfrm flipH="1" flipV="1">
           <a:off x="1514475" y="1009650"/>
           <a:ext cx="676275" cy="1971675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3514725" y="457200"/>
+          <a:ext cx="1409700" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1514475" y="666750"/>
+          <a:ext cx="1143000" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -693,26 +805,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G56"/>
+  <dimension ref="B2:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
@@ -721,6 +841,9 @@
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
@@ -729,6 +852,9 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
@@ -737,6 +863,9 @@
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1255,6 +1384,88 @@
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" s="1">
+        <v>10</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" s="1">
+        <v>10</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>